<commit_message>
Add Impediment Backlog Change Team Wiki
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Product Backlog.xlsx
+++ b/Document/SCRUM/Product Backlog.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Project Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Impediment Backlog" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>No.</t>
   </si>
@@ -125,13 +124,28 @@
   <si>
     <t>As the user, I want to use my webcam to made a video meeting with my doctor.
 So the information's exchange is more easier</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Group 2 Impediment</t>
+  </si>
+  <si>
+    <t>Some daily meeting late more than 20 minutes</t>
+  </si>
+  <si>
+    <t>Not solve</t>
+  </si>
+  <si>
+    <t>Not follow convention when commit code to SVN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +164,13 @@
     <font>
       <sz val="26"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,14 +196,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,35 +559,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -642,7 +668,7 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E9">
@@ -693,7 +719,7 @@
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E12">
@@ -713,7 +739,7 @@
       <c r="C13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E13">
@@ -730,7 +756,7 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G14">
@@ -790,7 +816,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -802,24 +828,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more task on Sprint Backlog.xlsx Update Group 2 Wiki.docx
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Product Backlog.xlsx
+++ b/Document/SCRUM/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Backlog" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>No.</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Not follow convention when commit code to SVN</t>
+  </si>
+  <si>
+    <t>When finish task, not commit to SVN for other member verify it</t>
   </si>
 </sst>
 </file>
@@ -242,8 +245,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G17" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:G17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G18" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:G18"/>
   <tableColumns count="7">
     <tableColumn id="1" name="No."/>
     <tableColumn id="2" name="Category"/>
@@ -544,17 +547,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -617,7 +620,10 @@
         <v>13</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>200</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -628,7 +634,10 @@
         <v>14</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>200</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,6 +821,11 @@
       </c>
       <c r="E17">
         <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -828,16 +842,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -878,6 +892,17 @@
       </c>
       <c r="C4" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Draft physical database] Add database diagram
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Product Backlog.xlsx
+++ b/Document/SCRUM/Product Backlog.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>No.</t>
   </si>
@@ -142,12 +142,81 @@
   </si>
   <si>
     <t>When finish task, not commit to SVN for other member verify it</t>
+  </si>
+  <si>
+    <t>Daily Meeting</t>
+  </si>
+  <si>
+    <t>13/05</t>
+  </si>
+  <si>
+    <t>14/5</t>
+  </si>
+  <si>
+    <t>Absent Without Plans</t>
+  </si>
+  <si>
+    <t>Absent With Plans</t>
+  </si>
+  <si>
+    <t>Tín</t>
+  </si>
+  <si>
+    <t>15/5</t>
+  </si>
+  <si>
+    <t>16/5</t>
+  </si>
+  <si>
+    <t>17/5</t>
+  </si>
+  <si>
+    <t>18/5</t>
+  </si>
+  <si>
+    <t>23/5</t>
+  </si>
+  <si>
+    <t>24/5</t>
+  </si>
+  <si>
+    <t>25/5</t>
+  </si>
+  <si>
+    <t>19/05</t>
+  </si>
+  <si>
+    <t>20/05</t>
+  </si>
+  <si>
+    <t>21/05</t>
+  </si>
+  <si>
+    <t>22/5</t>
+  </si>
+  <si>
+    <t>26/5</t>
+  </si>
+  <si>
+    <t>Dang</t>
+  </si>
+  <si>
+    <t>Tin</t>
+  </si>
+  <si>
+    <t>27/05</t>
+  </si>
+  <si>
+    <t>28/05</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="dd/mm"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -212,6 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,26 +912,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -872,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -883,7 +954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -894,7 +965,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -903,6 +974,121 @@
       </c>
       <c r="C5" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Fix Physical Database Diagram]
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Product Backlog.xlsx
+++ b/Document/SCRUM/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Project Backlog" sheetId="1" r:id="rId1"/>
@@ -215,7 +215,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm"/>
+    <numFmt numFmtId="164" formatCode="dd/mm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -275,13 +275,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,15 +632,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,11 +926,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -988,7 +988,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C16" t="s">
@@ -996,7 +996,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C17" t="s">
@@ -1004,17 +1004,17 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C20" t="s">
@@ -1022,12 +1022,12 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D22" t="s">
@@ -1035,7 +1035,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C23" t="s">
@@ -1043,7 +1043,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C24" t="s">
@@ -1051,22 +1051,22 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D28" t="s">
@@ -1074,7 +1074,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D29" t="s">
@@ -1082,12 +1082,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create sprint backlog, product backlog
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Product Backlog.xlsx
+++ b/Document/SCRUM/Product Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Project Backlog" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
   <si>
     <t>No.</t>
   </si>
@@ -26,30 +26,18 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>OMCS Product Backlog</t>
   </si>
   <si>
     <t>As the doctor, I want to create medical profile for patient</t>
   </si>
   <si>
-    <t>As the user, I want to login to the system</t>
-  </si>
-  <si>
     <t>As the PO, I want to see the basic design of system</t>
   </si>
   <si>
-    <t>Chat realtime</t>
-  </si>
-  <si>
     <t>Create medical profile</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Basic design</t>
   </si>
   <si>
@@ -83,26 +71,10 @@
     <t>Document</t>
   </si>
   <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Risk</t>
-  </si>
-  <si>
     <t>Design</t>
   </si>
   <si>
     <t>Team document</t>
-  </si>
-  <si>
-    <t>As a developer, I want to have some document 
-(product backlog, sprint backlog) created. So I can work well on OMCS</t>
-  </si>
-  <si>
-    <t>Project skeleton</t>
-  </si>
-  <si>
-    <t>As a developer, I want run OMCS successful on my computer</t>
   </si>
   <si>
     <t>Sprint</t>
@@ -112,20 +84,6 @@
 So I can send message and doctor receive immediately</t>
   </si>
   <si>
-    <t>Send image in chat conversation</t>
-  </si>
-  <si>
-    <t>As the user, I want to attach image and send to doctor.
-So the doctor can see it immediately.</t>
-  </si>
-  <si>
-    <t>Chat with video stream</t>
-  </si>
-  <si>
-    <t>As the user, I want to use my webcam to made a video meeting with my doctor.
-So the information's exchange is more easier</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -211,6 +169,137 @@
   </si>
   <si>
     <t>29/05</t>
+  </si>
+  <si>
+    <t>Acceptance criteria</t>
+  </si>
+  <si>
+    <t>As a team member, I want to have the introduction about the project so that I can understand the initial idea.</t>
+  </si>
+  <si>
+    <t>Delivery date</t>
+  </si>
+  <si>
+    <t>As a team member, I want to have the Project Management Plan so that I can work well on the project</t>
+  </si>
+  <si>
+    <t>20 May, 2014</t>
+  </si>
+  <si>
+    <t>The report should follow the template from FPT University
+Good layout, cover all items</t>
+  </si>
+  <si>
+    <t>As a team member, I want to have the System Requirements Specifications</t>
+  </si>
+  <si>
+    <t>As a team member, I want to have the System Design Specifications so that I can have a good design to follow</t>
+  </si>
+  <si>
+    <t>The report should follow the template from FPT University
+Good layout, cover all items
+All features are listed out and analysed carefully</t>
+  </si>
+  <si>
+    <t>As a team member, I want to have System Implementation &amp; Test document so that I can have full-featured and well-tested release</t>
+  </si>
+  <si>
+    <t>05 June, 2014</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>12 June, 2014</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>4, 5, 6, 7, 8</t>
+  </si>
+  <si>
+    <t>09 July, 2014</t>
+  </si>
+  <si>
+    <t>9, 10</t>
+  </si>
+  <si>
+    <t>As a team member, I want to have some document 
+(product backlog, sprint backlog, team wiki) created. So I can work well on OMCS</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>[User] Login</t>
+  </si>
+  <si>
+    <t>As a user, I want to login to the system</t>
+  </si>
+  <si>
+    <t>[User] Login with remember me</t>
+  </si>
+  <si>
+    <t>As a user, I want to login automatically</t>
+  </si>
+  <si>
+    <t>[User] Register</t>
+  </si>
+  <si>
+    <t>[User] Forget password</t>
+  </si>
+  <si>
+    <t>As a guest, I want to register new account</t>
+  </si>
+  <si>
+    <t>As a user, I want to get new password by email when I forgot it, so that I can continue to use OMCS</t>
+  </si>
+  <si>
+    <t>[User] Edit profile information</t>
+  </si>
+  <si>
+    <t>As a user, I want to update some information (profile picture, firstname,…)</t>
+  </si>
+  <si>
+    <t>[Patient] Update patient information</t>
+  </si>
+  <si>
+    <t>As a patient, I want to update some information about my profile, basic health record</t>
+  </si>
+  <si>
+    <t>For user experience, use in-place editor to edit information</t>
+  </si>
+  <si>
+    <t>[Patient] Chat</t>
+  </si>
+  <si>
+    <t>The behavior could be:
+The system list out all doctors with their status
+Patient can select doctor to chat with
+Patient can see old chat content</t>
+  </si>
+  <si>
+    <t>[Patient] Share webcam</t>
+  </si>
+  <si>
+    <t>Doctor can see the stream that patient share
+Doctor can see the stream in full-screen</t>
+  </si>
+  <si>
+    <t>[Patient] Attachment</t>
+  </si>
+  <si>
+    <t>As a patient, I want to attach some files, images and send to doctor</t>
+  </si>
+  <si>
+    <t>If attach files are images, display on the chat content, otherwise, let doctor download it</t>
+  </si>
+  <si>
+    <t>As a patient, I want to share my webcam so the information's exchange is more easier</t>
+  </si>
+  <si>
+    <t>[Admin] Define medical profile template</t>
   </si>
 </sst>
 </file>
@@ -259,7 +348,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -267,11 +356,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -285,11 +394,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -318,15 +444,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G18" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:G18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G19" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A2:G19"/>
   <tableColumns count="7">
     <tableColumn id="1" name="No."/>
     <tableColumn id="2" name="Category"/>
     <tableColumn id="3" name="Userstory"/>
-    <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Value"/>
-    <tableColumn id="6" name="Risk"/>
+    <tableColumn id="4" name="Description" dataDxfId="0"/>
+    <tableColumn id="6" name="Acceptance criteria"/>
+    <tableColumn id="7" name="Delivery date"/>
     <tableColumn id="8" name="Sprint"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -620,27 +746,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="59.5703125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="59.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -650,89 +778,125 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>200</v>
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>200</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>200</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,22 +904,25 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9">
-        <v>200</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9">
         <v>1</v>
       </c>
@@ -765,16 +932,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10">
-        <v>100</v>
+        <v>70</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -785,31 +949,24 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>20</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12">
         <v>1</v>
       </c>
@@ -819,92 +976,146 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>20</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="G13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
       <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
@@ -917,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +1141,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -940,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -951,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,10 +1173,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,133 +1184,133 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>